<commit_message>
foutjes in code aangepast
</commit_message>
<xml_diff>
--- a/v0.95-levensonderhoud-behandelen-Entiteiten-Attributen.xlsx
+++ b/v0.95-levensonderhoud-behandelen-Entiteiten-Attributen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vvng-my.sharepoint.com/personal/jan_brinkkemper_vng_nl/Documents/Publicatie-EA/Imvertor/Modellen op Github/koppelvlakken/Levensonderhoud-behandelen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{C3C4169C-0EB4-49B5-9316-841F6E8656E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{103FE98F-E16B-447B-B958-67EAC6C6862E}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="8_{C3C4169C-0EB4-49B5-9316-841F6E8656E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9167989B-F444-4F8E-82CD-B890355C6ECE}"/>
   <bookViews>
-    <workbookView xWindow="3430" yWindow="340" windowWidth="17620" windowHeight="11370" xr2:uid="{459DC88B-0BB4-4CC7-BB02-9EC2264ADF87}"/>
+    <workbookView xWindow="8060" yWindow="3160" windowWidth="27060" windowHeight="18100" xr2:uid="{459DC88B-0BB4-4CC7-BB02-9EC2264ADF87}"/>
   </bookViews>
   <sheets>
     <sheet name="LO Behandelen" sheetId="1" r:id="rId1"/>
@@ -634,9 +634,6 @@
     <t>IndicatieInstellingVolledigVerzorgd</t>
   </si>
   <si>
-    <t>V0.94</t>
-  </si>
-  <si>
     <t>Alimentatie</t>
   </si>
   <si>
@@ -691,6 +688,9 @@
   </si>
   <si>
     <t>1-Ja 2-Nee 8-Niet van toepassing</t>
+  </si>
+  <si>
+    <t>V0.95</t>
   </si>
 </sst>
 </file>
@@ -1113,8 +1113,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1290,38 +1290,38 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" t="s">
         <v>196</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>197</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>208</v>
-      </c>
       <c r="D16" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1704,7 +1704,7 @@
         <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2041,7 +2041,7 @@
         <v>5</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -2113,7 +2113,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B90" t="s">
         <v>122</v>
@@ -2138,13 +2138,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
+        <v>199</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" t="s">
         <v>200</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F92" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -2316,7 +2316,7 @@
         <v>116</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>21</v>
@@ -2360,7 +2360,7 @@
         <v>5</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -2380,7 +2380,7 @@
         <v>78</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D113" s="7" t="s">
         <v>4</v>
@@ -2424,7 +2424,7 @@
         <v>4</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>